<commit_message>
Alterando planilha para escopo de testes
</commit_message>
<xml_diff>
--- a/src/main/resources/EntradasPW1.xlsx
+++ b/src/main/resources/EntradasPW1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="35">
   <si>
     <t xml:space="preserve">2226</t>
   </si>
@@ -445,7 +445,7 @@
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AJ10" activeCellId="0" sqref="AJ10"/>
+      <selection pane="topLeft" activeCell="AI23" activeCellId="0" sqref="AI23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1443,7 +1443,7 @@
         <v>18</v>
       </c>
       <c r="AC17" s="8" t="n">
-        <v>300.6</v>
+        <v>300.5</v>
       </c>
       <c r="AD17" s="7" t="n">
         <v>0</v>
@@ -1454,7 +1454,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>1866</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>45862</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="2" t="n">
+        <v>36</v>
+      </c>
+      <c r="K18" s="2" t="n">
+        <v>73</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18" s="6" t="n">
+        <v>1101</v>
+      </c>
+      <c r="Q18" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="U18" s="7" t="n">
+        <v>1670</v>
+      </c>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z18" s="8" t="n">
+        <v>1670</v>
+      </c>
+      <c r="AB18" s="9" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC18" s="8" t="n">
+        <v>200</v>
+      </c>
+      <c r="AD18" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="7"/>
+      <c r="AF18" s="7"/>
+      <c r="AH18" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2198,7 +2254,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="34">
+  <mergeCells count="36">
     <mergeCell ref="U1:W1"/>
     <mergeCell ref="AD1:AF1"/>
     <mergeCell ref="U2:W2"/>
@@ -2233,6 +2289,8 @@
     <mergeCell ref="AD16:AF16"/>
     <mergeCell ref="U17:W17"/>
     <mergeCell ref="AD17:AF17"/>
+    <mergeCell ref="U18:W18"/>
+    <mergeCell ref="AD18:AF18"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.747916666666667" top="1" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>